<commit_message>
Data source documentation update
</commit_message>
<xml_diff>
--- a/Documentation/Data Source Spreadsheet.xlsx
+++ b/Documentation/Data Source Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Downloads\Github Repos\rstudy-edu\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF7FF63-5196-4374-B38A-C09D0DB3FD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FD6F79-DE98-4D36-8808-50938BC1DA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{354D6AAB-0683-442D-824C-947A5389DE34}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{354D6AAB-0683-442D-824C-947A5389DE34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Dataset Source</t>
   </si>
@@ -291,6 +291,15 @@
   </si>
   <si>
     <t>EDFacts from the US Department of Education</t>
+  </si>
+  <si>
+    <t>https://nces.ed.gov/ccd/Data/zip/sdf22_1a_sas7bdat.zip</t>
+  </si>
+  <si>
+    <t>https://assets.ctfassets.net/9fbw4onh0qc1/51GumHMBAalCkUBBHREfxO/0f4e84f44f90451b5558e7989e0d342b/CSDH_Introductory_White_Paper.pdf</t>
+  </si>
+  <si>
+    <t>https://www.lee.senate.gov/services/files/DA64FDB7-3B2E-40D4-B9E3-07001B81EC31</t>
   </si>
 </sst>
 </file>
@@ -678,11 +687,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A579C8-599B-480C-8906-491CCEFE5A0F}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,10 +704,11 @@
     <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="24.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="18.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -727,7 +737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -756,7 +766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -787,8 +797,11 @@
       <c r="J3" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -811,7 +824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -834,7 +847,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -859,8 +872,11 @@
       <c r="H6" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -886,7 +902,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -909,7 +925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
@@ -931,8 +947,11 @@
       <c r="H9" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -958,7 +977,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -984,7 +1003,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>79</v>
       </c>
@@ -1020,24 +1039,24 @@
     <hyperlink ref="F4" r:id="rId9" xr:uid="{90655C90-5067-4A08-8F1C-9021820C3591}"/>
     <hyperlink ref="E5" r:id="rId10" xr:uid="{BEC4D25E-1FD4-4C83-8EA6-3F6CB111D650}"/>
     <hyperlink ref="F6" r:id="rId11" xr:uid="{F6409C84-FCB9-478F-A54E-9F93BF124218}"/>
-    <hyperlink ref="E6" r:id="rId12" xr:uid="{C14D39CF-7FB3-432B-8FB1-341FF2ED360E}"/>
-    <hyperlink ref="G6" r:id="rId13" xr:uid="{F96DBF60-921E-4EE4-AF73-EE759F92C379}"/>
-    <hyperlink ref="F7" r:id="rId14" xr:uid="{EEEDA093-A5B6-4DAA-BBAB-1B00D70F2F40}"/>
-    <hyperlink ref="E7" r:id="rId15" xr:uid="{EE999172-4E1A-414D-B687-EF4C083A096A}"/>
-    <hyperlink ref="G7" r:id="rId16" xr:uid="{99D80737-2FBD-49FE-A959-55829714BE76}"/>
-    <hyperlink ref="F8" r:id="rId17" xr:uid="{EC709CC3-A152-476A-A499-679AB97E1E61}"/>
-    <hyperlink ref="E8" r:id="rId18" xr:uid="{FCEACE5D-FE18-4F2B-9E24-62ED658A4433}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{F2680D27-F16C-4E1C-BE61-F3950C823C1A}"/>
-    <hyperlink ref="E9" r:id="rId20" xr:uid="{D4F6D1DE-7FBE-4DB6-82A3-D3E65F33DA85}"/>
-    <hyperlink ref="E10" r:id="rId21" xr:uid="{9D86A22E-2274-4A40-B089-99104E14B683}"/>
-    <hyperlink ref="F10" r:id="rId22" location="resource-listing" xr:uid="{E539CFBE-EB0F-4B77-B5DB-841ED64639AC}"/>
-    <hyperlink ref="G10" r:id="rId23" xr:uid="{D7C88BEF-27B9-47D3-8E26-B71868D2C136}"/>
-    <hyperlink ref="E11" r:id="rId24" xr:uid="{999386BB-0742-45CF-9134-21A8E1CE14C1}"/>
-    <hyperlink ref="F11" r:id="rId25" xr:uid="{7D963D7B-5A12-4C79-814E-9CD95E6967D5}"/>
-    <hyperlink ref="G11" r:id="rId26" xr:uid="{496647E8-2EEE-4432-B488-4CF72C38F90B}"/>
-    <hyperlink ref="E12" r:id="rId27" xr:uid="{DB593B2B-0BDB-4378-8E99-08CA3C58DC58}"/>
-    <hyperlink ref="F12" r:id="rId28" xr:uid="{A637ACD5-1585-4832-9F70-18BE582FE155}"/>
-    <hyperlink ref="G12" r:id="rId29" xr:uid="{DB2D2652-1D1A-4D71-8634-EA3B040B1F52}"/>
+    <hyperlink ref="G6" r:id="rId12" xr:uid="{F96DBF60-921E-4EE4-AF73-EE759F92C379}"/>
+    <hyperlink ref="F7" r:id="rId13" xr:uid="{EEEDA093-A5B6-4DAA-BBAB-1B00D70F2F40}"/>
+    <hyperlink ref="E7" r:id="rId14" xr:uid="{EE999172-4E1A-414D-B687-EF4C083A096A}"/>
+    <hyperlink ref="G7" r:id="rId15" xr:uid="{99D80737-2FBD-49FE-A959-55829714BE76}"/>
+    <hyperlink ref="F8" r:id="rId16" xr:uid="{EC709CC3-A152-476A-A499-679AB97E1E61}"/>
+    <hyperlink ref="E8" r:id="rId17" xr:uid="{FCEACE5D-FE18-4F2B-9E24-62ED658A4433}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{F2680D27-F16C-4E1C-BE61-F3950C823C1A}"/>
+    <hyperlink ref="E9" r:id="rId19" xr:uid="{D4F6D1DE-7FBE-4DB6-82A3-D3E65F33DA85}"/>
+    <hyperlink ref="E10" r:id="rId20" xr:uid="{9D86A22E-2274-4A40-B089-99104E14B683}"/>
+    <hyperlink ref="F10" r:id="rId21" location="resource-listing" xr:uid="{E539CFBE-EB0F-4B77-B5DB-841ED64639AC}"/>
+    <hyperlink ref="G10" r:id="rId22" xr:uid="{D7C88BEF-27B9-47D3-8E26-B71868D2C136}"/>
+    <hyperlink ref="E11" r:id="rId23" xr:uid="{999386BB-0742-45CF-9134-21A8E1CE14C1}"/>
+    <hyperlink ref="F11" r:id="rId24" xr:uid="{7D963D7B-5A12-4C79-814E-9CD95E6967D5}"/>
+    <hyperlink ref="G11" r:id="rId25" xr:uid="{496647E8-2EEE-4432-B488-4CF72C38F90B}"/>
+    <hyperlink ref="E12" r:id="rId26" xr:uid="{DB593B2B-0BDB-4378-8E99-08CA3C58DC58}"/>
+    <hyperlink ref="F12" r:id="rId27" xr:uid="{A637ACD5-1585-4832-9F70-18BE582FE155}"/>
+    <hyperlink ref="G12" r:id="rId28" xr:uid="{DB2D2652-1D1A-4D71-8634-EA3B040B1F52}"/>
+    <hyperlink ref="E6" r:id="rId29" xr:uid="{C14D39CF-7FB3-432B-8FB1-341FF2ED360E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId30"/>

</xml_diff>